<commit_message>
brief blurb about Euler's identity
</commit_message>
<xml_diff>
--- a/PlyCB.protein.quantifications.calculations.one.phase.decay.xlsx
+++ b/PlyCB.protein.quantifications.calculations.one.phase.decay.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\NelsonShared\Harley\NelsonLab_EXPERIMENTS\Exp722\PlyCB.Bradford.quantification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\NelsonShared\Harley\NelsonLab_EXPERIMENTS\Exp722\PlyCB.Bradford.quantification\Bradford-Assay-Protein-Quant-with-One-Phase-Assoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E1F886-E87B-4EEE-BAAD-BED80C3489BB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC87EDA1-DA80-493C-BD00-ED27883A2DB6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="945" yWindow="0" windowWidth="27855" windowHeight="12750" xr2:uid="{D3F9AF53-D4C9-4726-A6E1-E3A683F5745C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="83">
   <si>
     <t>Used Bradford assay to quantify PlyCB protein concentration.</t>
   </si>
@@ -271,6 +271,15 @@
   </si>
   <si>
     <t>abs</t>
+  </si>
+  <si>
+    <t>Why 2ipin?</t>
+  </si>
+  <si>
+    <t>related to integers and Euler's identity. Here, can use n = 0.</t>
+  </si>
+  <si>
+    <t>https://www.quora.com/If-e-2-pi-i-1-does-this-mean-that-e-2-pi-i-e-0-So-2-pi-i-0</t>
   </si>
 </sst>
 </file>
@@ -1256,7 +1265,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63E47F21-8D58-44FA-ACA0-95E2F447855C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1297,7 +1306,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94BEACAA-FD0B-4A98-8F49-09A6F33D9BCF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1318,23 +1327,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1360,7 +1356,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F927411E-5402-4747-BA01-B83F84723F8D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1404,7 +1400,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{723A556A-4BBF-4E0F-A51F-1E0E1BDA8E9B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1733,7 +1729,7 @@
   <dimension ref="A1:U102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G87" sqref="G87"/>
+      <selection activeCell="H89" sqref="H89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3091,6 +3087,9 @@
         <v>54</v>
       </c>
       <c r="E87" s="4"/>
+      <c r="G87" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="88" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C88" s="2" t="s">
@@ -3100,6 +3099,9 @@
         <v>55</v>
       </c>
       <c r="E88" s="4"/>
+      <c r="G88" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="89" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C89" s="2" t="s">
@@ -3109,6 +3111,9 @@
         <v>56</v>
       </c>
       <c r="E89" s="4"/>
+      <c r="G89" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="90" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C90" s="2" t="s">

</xml_diff>